<commit_message>
added new input file
</commit_message>
<xml_diff>
--- a/test_files/CS520_2019_Project1_Test_Cases.xlsx
+++ b/test_files/CS520_2019_Project1_Test_Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adita\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeStuff\OutOfOrderSimulator\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25436D1-7290-46E2-9EA6-F96350BBE78F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA003DF-7A56-4A6B-AE6D-DD1F6CAAF19F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="711" xr2:uid="{ECC43C12-43ED-43C3-8B7A-AC83D851DE0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="711" activeTab="2" xr2:uid="{ECC43C12-43ED-43C3-8B7A-AC83D851DE0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic without forwarding" sheetId="4" r:id="rId1"/>
@@ -1434,44 +1434,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075FFD27-2241-4F29-91DD-7CA5483E777A}">
   <dimension ref="B1:CE27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="5.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="7" max="7" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="2.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="28" width="3.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.88671875" style="4" customWidth="1"/>
-    <col min="31" max="32" width="3.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="3.88671875" style="4" customWidth="1"/>
-    <col min="35" max="39" width="3.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="3.88671875" style="4" customWidth="1"/>
-    <col min="41" max="52" width="3.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.33203125" style="4" customWidth="1"/>
-    <col min="54" max="54" width="4.109375" style="4" customWidth="1"/>
-    <col min="55" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.85546875" style="4"/>
+    <col min="2" max="2" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="4"/>
+    <col min="7" max="7" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="2.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="28" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.85546875" style="4" customWidth="1"/>
+    <col min="31" max="32" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="3.85546875" style="4" customWidth="1"/>
+    <col min="35" max="39" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.85546875" style="4" customWidth="1"/>
+    <col min="41" max="52" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="4.140625" style="4" customWidth="1"/>
+    <col min="55" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:83" x14ac:dyDescent="0.25">
       <c r="D1" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B2" s="66" t="s">
         <v>97</v>
       </c>
@@ -1619,7 +1619,7 @@
       <c r="BA2" s="26"/>
       <c r="BB2" s="26"/>
     </row>
-    <row r="3" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="27">
         <v>4000</v>
       </c>
@@ -1761,7 +1761,7 @@
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
     </row>
-    <row r="4" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="27">
         <v>4004</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
     </row>
-    <row r="5" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" s="27">
         <v>4008</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
     </row>
-    <row r="6" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="27">
         <v>4012</v>
       </c>
@@ -2097,7 +2097,7 @@
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
     </row>
-    <row r="7" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="27">
         <v>4016</v>
       </c>
@@ -2195,7 +2195,7 @@
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
     </row>
-    <row r="8" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
         <v>4020</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="CD8" s="41"/>
       <c r="CE8" s="41"/>
     </row>
-    <row r="9" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>4024</v>
       </c>
@@ -2427,7 +2427,7 @@
       <c r="BD9" s="41"/>
       <c r="BE9" s="41"/>
     </row>
-    <row r="10" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>4028</v>
       </c>
@@ -2475,7 +2475,7 @@
       <c r="AT10" s="60"/>
       <c r="AU10" s="60"/>
     </row>
-    <row r="11" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>4032</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>4036</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <v>4040</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
         <v>4044</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="15" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>4048</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:83" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>4052</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>4056</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>4060</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
         <v>4064</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="27">
         <v>4068</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
         <v>4072</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>4076</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G23" s="2" t="s">
         <v>85</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="23"/>
       <c r="D24" s="2" t="s">
         <v>135</v>
@@ -2742,7 +2742,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" s="43"/>
       <c r="D25" s="2" t="s">
         <v>131</v>
@@ -2754,7 +2754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26" s="24" t="s">
         <v>92</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G27" s="2" t="s">
         <v>89</v>
       </c>
@@ -2794,35 +2794,35 @@
       <selection pane="topRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="31" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="42" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="53" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="54" max="84" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="31" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="42" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="53" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="84" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="60" t="s">
         <v>166</v>
       </c>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="70" t="s">
         <v>95</v>
       </c>
@@ -2837,7 +2837,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>4000</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>4004</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4008</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4012</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4016</v>
       </c>
@@ -2993,7 +2993,7 @@
       <c r="Q7" s="21"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4020</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="Q8" s="21"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4024</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="Q9" s="21"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>4028</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="Q10" s="21"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4032</v>
       </c>
@@ -3129,7 +3129,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>4036</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>4040</v>
       </c>
@@ -3185,7 +3185,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>4044</v>
       </c>
@@ -3213,7 +3213,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>4048</v>
       </c>
@@ -3241,7 +3241,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="2:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>4052</v>
       </c>
@@ -3271,7 +3271,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>4056</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4060</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>4064</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>4068</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>4072</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>4076</v>
       </c>
@@ -3401,7 +3401,7 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="24" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="67" t="s">
         <v>46</v>
       </c>
@@ -3446,7 +3446,7 @@
       <c r="AM24" s="4"/>
       <c r="AN24" s="4"/>
     </row>
-    <row r="25" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
@@ -3703,7 +3703,7 @@
       <c r="CK25" s="8"/>
       <c r="CL25" s="8"/>
     </row>
-    <row r="26" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="CE26" s="9"/>
       <c r="CF26" s="9"/>
     </row>
-    <row r="27" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="CE27" s="9"/>
       <c r="CF27" s="9"/>
     </row>
-    <row r="28" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>54</v>
       </c>
@@ -4338,7 +4338,7 @@
       <c r="CE28" s="9"/>
       <c r="CF28" s="9"/>
     </row>
-    <row r="29" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>51</v>
       </c>
@@ -4495,7 +4495,7 @@
       <c r="CE29" s="9"/>
       <c r="CF29" s="9"/>
     </row>
-    <row r="30" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>52</v>
       </c>
@@ -4652,7 +4652,7 @@
       <c r="CE30" s="9"/>
       <c r="CF30" s="9"/>
     </row>
-    <row r="31" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>53</v>
       </c>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="CF31" s="9"/>
     </row>
-    <row r="32" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>50</v>
       </c>
@@ -4966,21 +4966,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="17"/>
       <c r="D35" s="68" t="s">
         <v>67</v>
       </c>
       <c r="E35" s="68"/>
     </row>
-    <row r="36" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="7"/>
       <c r="D36" s="68" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="68"/>
     </row>
-    <row r="37" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="18"/>
       <c r="D37" s="69" t="s">
         <v>69</v>
@@ -5005,38 +5005,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98ECD635-F5C2-4ECB-9159-5B8013948045}">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="44"/>
-    <col min="2" max="2" width="5.44140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="44"/>
-    <col min="8" max="8" width="7.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.77734375" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="2.77734375" style="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="44"/>
+    <col min="2" max="2" width="5.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="44"/>
+    <col min="8" max="8" width="7.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="2.7109375" style="44" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5" style="44" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.77734375" style="44" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="3.88671875" style="44" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="3.88671875" style="44" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="27" max="35" width="3.88671875" style="44" bestFit="1" customWidth="1"/>
-    <col min="36" max="1024" width="8.88671875" style="44"/>
+    <col min="17" max="17" width="2.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="3.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="3.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="27" max="35" width="3.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="36" max="1024" width="8.85546875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="60" t="s">
@@ -5075,7 +5075,7 @@
       <c r="AJ1"/>
       <c r="AK1"/>
     </row>
-    <row r="2" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B2" s="73" t="s">
         <v>136</v>
       </c>
@@ -5185,7 +5185,7 @@
       <c r="AY2" s="26"/>
       <c r="AZ2" s="26"/>
     </row>
-    <row r="3" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="27">
         <v>4000</v>
       </c>
@@ -5291,7 +5291,7 @@
       <c r="AY3" s="26"/>
       <c r="AZ3" s="26"/>
     </row>
-    <row r="4" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="27">
         <v>4004</v>
       </c>
@@ -5393,7 +5393,7 @@
       <c r="AY4" s="26"/>
       <c r="AZ4" s="26"/>
     </row>
-    <row r="5" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" s="27">
         <v>4008</v>
       </c>
@@ -5489,7 +5489,7 @@
       <c r="AY5" s="26"/>
       <c r="AZ5" s="26"/>
     </row>
-    <row r="6" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="27">
         <v>4012</v>
       </c>
@@ -5583,7 +5583,7 @@
       <c r="AY6" s="26"/>
       <c r="AZ6" s="26"/>
     </row>
-    <row r="7" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="27">
         <v>4016</v>
       </c>
@@ -5677,7 +5677,7 @@
       <c r="AY7" s="26"/>
       <c r="AZ7" s="26"/>
     </row>
-    <row r="8" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
         <v>4020</v>
       </c>
@@ -5771,7 +5771,7 @@
       <c r="AY8" s="26"/>
       <c r="AZ8" s="50"/>
     </row>
-    <row r="9" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>4024</v>
       </c>
@@ -5865,7 +5865,7 @@
       <c r="AY9" s="26"/>
       <c r="AZ9" s="26"/>
     </row>
-    <row r="10" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>4028</v>
       </c>
@@ -5925,7 +5925,7 @@
       <c r="AY10" s="4"/>
       <c r="AZ10" s="4"/>
     </row>
-    <row r="11" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>4032</v>
       </c>
@@ -5985,7 +5985,7 @@
       <c r="AY11" s="4"/>
       <c r="AZ11" s="4"/>
     </row>
-    <row r="12" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>4036</v>
       </c>
@@ -6053,7 +6053,7 @@
       <c r="AY12" s="4"/>
       <c r="AZ12" s="4"/>
     </row>
-    <row r="13" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <v>4040</v>
       </c>
@@ -6121,7 +6121,7 @@
       <c r="AY13" s="4"/>
       <c r="AZ13" s="4"/>
     </row>
-    <row r="14" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
         <v>4044</v>
       </c>
@@ -6185,7 +6185,7 @@
       <c r="AY14" s="4"/>
       <c r="AZ14" s="4"/>
     </row>
-    <row r="15" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>4048</v>
       </c>
@@ -6249,7 +6249,7 @@
       <c r="AY15" s="4"/>
       <c r="AZ15" s="4"/>
     </row>
-    <row r="16" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>4052</v>
       </c>
@@ -6313,7 +6313,7 @@
       <c r="AY16" s="4"/>
       <c r="AZ16" s="4"/>
     </row>
-    <row r="17" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>4056</v>
       </c>
@@ -6377,7 +6377,7 @@
       <c r="AY17" s="4"/>
       <c r="AZ17" s="4"/>
     </row>
-    <row r="18" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>4060</v>
       </c>
@@ -6441,7 +6441,7 @@
       <c r="AY18" s="4"/>
       <c r="AZ18" s="4"/>
     </row>
-    <row r="19" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
         <v>4064</v>
       </c>
@@ -6505,7 +6505,7 @@
       <c r="AY19" s="4"/>
       <c r="AZ19" s="4"/>
     </row>
-    <row r="20" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B20" s="27">
         <v>4068</v>
       </c>
@@ -6569,7 +6569,7 @@
       <c r="AY20" s="4"/>
       <c r="AZ20" s="4"/>
     </row>
-    <row r="21" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:52" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
         <v>4072</v>
       </c>
@@ -6631,7 +6631,7 @@
       <c r="AY21" s="4"/>
       <c r="AZ21" s="4"/>
     </row>
-    <row r="22" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>4076</v>
       </c>
@@ -6695,7 +6695,7 @@
       <c r="AY22" s="4"/>
       <c r="AZ22" s="4"/>
     </row>
-    <row r="23" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:52" x14ac:dyDescent="0.25">
       <c r="C23"/>
       <c r="D23"/>
       <c r="H23" s="2" t="s">
@@ -6748,7 +6748,7 @@
       <c r="AY23" s="4"/>
       <c r="AZ23" s="4"/>
     </row>
-    <row r="24" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:52" x14ac:dyDescent="0.25">
       <c r="C24" s="59"/>
       <c r="D24" s="47" t="s">
         <v>147</v>
@@ -6806,7 +6806,7 @@
       <c r="AY24" s="4"/>
       <c r="AZ24" s="4"/>
     </row>
-    <row r="25" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:52" x14ac:dyDescent="0.25">
       <c r="C25" s="53"/>
       <c r="D25" s="47" t="s">
         <v>148</v>
@@ -6861,7 +6861,7 @@
       <c r="AY25" s="4"/>
       <c r="AZ25" s="4"/>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:52" x14ac:dyDescent="0.25">
       <c r="C26" s="54"/>
       <c r="D26" s="47" t="s">
         <v>67</v>
@@ -6916,7 +6916,7 @@
       <c r="AY26" s="4"/>
       <c r="AZ26" s="4"/>
     </row>
-    <row r="27" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:52" x14ac:dyDescent="0.25">
       <c r="C27" s="55" t="s">
         <v>92</v>
       </c>
@@ -6973,7 +6973,7 @@
       <c r="AY27" s="4"/>
       <c r="AZ27" s="4"/>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:52" x14ac:dyDescent="0.25">
       <c r="C28" s="57"/>
       <c r="D28" s="47" t="s">
         <v>161</v>
@@ -6996,34 +6996,34 @@
       <selection pane="topRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="3.21875" bestFit="1" customWidth="1"/>
-    <col min="39" max="84" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="84" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="60" t="s">
         <v>166</v>
       </c>
       <c r="E1" s="61"/>
     </row>
-    <row r="2" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="74" t="s">
         <v>96</v>
       </c>
@@ -7037,7 +7037,7 @@
       <c r="P2" s="61"/>
       <c r="Q2" s="61"/>
     </row>
-    <row r="3" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>4000</v>
       </c>
@@ -7070,7 +7070,7 @@
       <c r="R3" s="63"/>
       <c r="S3" s="64"/>
     </row>
-    <row r="4" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>4004</v>
       </c>
@@ -7103,7 +7103,7 @@
       <c r="R4" s="63"/>
       <c r="S4" s="64"/>
     </row>
-    <row r="5" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4008</v>
       </c>
@@ -7136,7 +7136,7 @@
       <c r="R5" s="63"/>
       <c r="S5" s="64"/>
     </row>
-    <row r="6" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4012</v>
       </c>
@@ -7168,7 +7168,7 @@
       </c>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4016</v>
       </c>
@@ -7195,7 +7195,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="21"/>
     </row>
-    <row r="8" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4020</v>
       </c>
@@ -7228,7 +7228,7 @@
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
     </row>
-    <row r="9" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4024</v>
       </c>
@@ -7261,7 +7261,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
     </row>
-    <row r="10" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>4028</v>
       </c>
@@ -7294,7 +7294,7 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
     </row>
-    <row r="11" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4032</v>
       </c>
@@ -7327,7 +7327,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>4036</v>
       </c>
@@ -7354,7 +7354,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>4040</v>
       </c>
@@ -7381,7 +7381,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>4044</v>
       </c>
@@ -7408,7 +7408,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>4048</v>
       </c>
@@ -7435,7 +7435,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>4052</v>
       </c>
@@ -7464,7 +7464,7 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>4056</v>
       </c>
@@ -7493,7 +7493,7 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4060</v>
       </c>
@@ -7522,7 +7522,7 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>4064</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>4068</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>4072</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>4076</v>
       </c>
@@ -7592,7 +7592,7 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="24" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="67" t="s">
         <v>94</v>
       </c>
@@ -7637,7 +7637,7 @@
       <c r="AM24" s="4"/>
       <c r="AN24" s="4"/>
     </row>
-    <row r="25" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
@@ -7849,7 +7849,7 @@
       <c r="CK25" s="8"/>
       <c r="CL25" s="8"/>
     </row>
-    <row r="26" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
@@ -8022,7 +8022,7 @@
       <c r="BI26" s="9"/>
       <c r="BJ26" s="9"/>
     </row>
-    <row r="27" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
@@ -8187,7 +8187,7 @@
       <c r="BI27" s="9"/>
       <c r="BJ27" s="9"/>
     </row>
-    <row r="28" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>54</v>
       </c>
@@ -8330,7 +8330,7 @@
       <c r="BI28" s="9"/>
       <c r="BJ28" s="9"/>
     </row>
-    <row r="29" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>51</v>
       </c>
@@ -8465,7 +8465,7 @@
       <c r="BI29" s="9"/>
       <c r="BJ29" s="9"/>
     </row>
-    <row r="30" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>52</v>
       </c>
@@ -8600,7 +8600,7 @@
       <c r="BI30" s="9"/>
       <c r="BJ30" s="9"/>
     </row>
-    <row r="31" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>53</v>
       </c>
@@ -8735,7 +8735,7 @@
       </c>
       <c r="BJ31" s="9"/>
     </row>
-    <row r="32" spans="2:90" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:90" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>50</v>
       </c>
@@ -8870,21 +8870,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="17"/>
       <c r="D35" s="68" t="s">
         <v>67</v>
       </c>
       <c r="E35" s="68"/>
     </row>
-    <row r="36" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="7"/>
       <c r="D36" s="68" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="68"/>
     </row>
-    <row r="37" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="18"/>
       <c r="D37" s="69" t="s">
         <v>69</v>

</xml_diff>